<commit_message>
tested with a response as well
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -375,38 +375,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>name</v>
+        <v>id</v>
       </c>
       <c r="B1" t="str">
-        <v>age</v>
+        <v>page_id</v>
+      </c>
+      <c r="C1" t="str">
+        <v>emotion</v>
+      </c>
+      <c r="D1" t="str">
+        <v>contact_details</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Guro</v>
-      </c>
-      <c r="B2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Elon</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
+        <v>b03e7319-7477-482f-96f2-cb89ddf0d08d</v>
+      </c>
+      <c r="B2" t="str">
+        <v>pageid</v>
+      </c>
+      <c r="C2" t="str">
+        <v>:-)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
playint around with query_
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -375,39 +375,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>id</v>
+        <v>a</v>
       </c>
       <c r="B1" t="str">
-        <v>page_id</v>
-      </c>
-      <c r="C1" t="str">
-        <v>emotion</v>
-      </c>
-      <c r="D1" t="str">
-        <v>contact_details</v>
+        <v>b</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>b03e7319-7477-482f-96f2-cb89ddf0d08d</v>
-      </c>
-      <c r="B2" t="str">
-        <v>pageid</v>
-      </c>
-      <c r="C2" t="str">
-        <v>:-)</v>
+        <v>first of a</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="str">
+        <v>first of b</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>second of only a</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>a of has both</v>
+      </c>
+      <c r="B5" t="str">
+        <v>b of has both</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>